<commit_message>
EB adding KNN test and outliers checks
also add add NALL to the dtatset
</commit_message>
<xml_diff>
--- a/result/Football_data_protocol.xlsx
+++ b/result/Football_data_protocol.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1039,6 +1039,18 @@
         </is>
       </c>
       <c r="B51" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>int64</t>
         </is>
@@ -1055,7 +1067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1572,6 +1584,16 @@
       </c>
       <c r="B51" t="n">
         <v>31</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1585,7 +1607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2102,6 +2124,16 @@
       </c>
       <c r="B51" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2115,7 +2147,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2627,6 +2659,16 @@
         </is>
       </c>
       <c r="B51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2641,7 +2683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3156,6 +3198,16 @@
         <v>31</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>